<commit_message>
Improvements to narrative layout Added groupings and grouping descriptions to the artifact index Added several documents types and few sections for the doc types
</commit_message>
<xml_diff>
--- a/docs/2.16.840.1.113883.10.20.22.1.1.xlsx
+++ b/docs/2.16.840.1.113883.10.20.22.1.1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="166">
   <si>
     <t>Path</t>
   </si>
@@ -272,6 +272,10 @@
     <t>SHALL contain exactly one [1..1] US Realm Date and Time (DTM.US.FIELDED) (identifier: urn:oid:2.16.840.1.113883.10.20.22.5.4) (CONF:1198-5256).</t>
   </si>
   <si>
+    <t>81-10127:**SHALL** be precise to the day (CONF:81-10127). {null}
+81-10128:**SHOULD** be precise to the minute (CONF:81-10128). {null}81-10129:**MAY** be precise to the second (CONF:81-10129). {null}81-10130:If more precise than day, **SHOULD** include time-zone offset (CONF:81-10130). {null}</t>
+  </si>
+  <si>
     <t>ClinicalDocument.confidentialityCode</t>
   </si>
   <si>
@@ -441,8 +445,8 @@
     <t>MAY contain zero or more [0..*] authenticator (CONF:1198-5607) such that it</t>
   </si>
   <si>
-    <t>value:ClinicalDocument.signatureCode}
-value:ClinicalDocument.assignedEntity}value:ClinicalDocument.time}</t>
+    <t xml:space="preserve">value:signatureCode}
+</t>
   </si>
   <si>
     <t>authenticator1</t>
@@ -725,7 +729,7 @@
     <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="45.51171875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="62.6875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="20.06640625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
@@ -1891,12 +1895,12 @@
         <v>36</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>36</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -1922,10 +1926,10 @@
         <v>70</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1976,7 +1980,7 @@
         <v>36</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>37</v>
@@ -1993,7 +1997,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2019,10 +2023,10 @@
         <v>51</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2073,7 +2077,7 @@
         <v>36</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>39</v>
@@ -2090,7 +2094,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2116,10 +2120,10 @@
         <v>56</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2170,7 +2174,7 @@
         <v>36</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>39</v>
@@ -2182,12 +2186,12 @@
         <v>36</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2210,13 +2214,13 @@
         <v>36</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2267,7 +2271,7 @@
         <v>36</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>39</v>
@@ -2279,12 +2283,12 @@
         <v>36</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2307,7 +2311,7 @@
         <v>36</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -2360,7 +2364,7 @@
         <v>36</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>39</v>
@@ -2377,7 +2381,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2400,13 +2404,13 @@
         <v>36</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2457,7 +2461,7 @@
         <v>36</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>37</v>
@@ -2474,7 +2478,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2497,13 +2501,13 @@
         <v>36</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2554,7 +2558,7 @@
         <v>36</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>37</v>
@@ -2571,7 +2575,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2594,13 +2598,13 @@
         <v>36</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2651,7 +2655,7 @@
         <v>36</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
@@ -2668,7 +2672,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -2691,11 +2695,11 @@
         <v>36</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2734,7 +2738,7 @@
         <v>36</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AB21" s="2"/>
       <c r="AC21" t="s" s="2">
@@ -2744,7 +2748,7 @@
         <v>62</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>39</v>
@@ -2761,10 +2765,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>36</v>
@@ -2786,13 +2790,13 @@
         <v>36</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -2843,7 +2847,7 @@
         <v>36</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
@@ -2860,10 +2864,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>36</v>
@@ -2885,13 +2889,13 @@
         <v>36</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2942,7 +2946,7 @@
         <v>36</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
@@ -2959,7 +2963,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -2982,13 +2986,13 @@
         <v>36</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3039,7 +3043,7 @@
         <v>36</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>37</v>
@@ -3056,7 +3060,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3079,13 +3083,13 @@
         <v>36</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -3136,7 +3140,7 @@
         <v>36</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3153,7 +3157,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3176,13 +3180,13 @@
         <v>36</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -3233,7 +3237,7 @@
         <v>36</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>39</v>
@@ -3250,7 +3254,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3273,11 +3277,11 @@
         <v>36</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -3316,7 +3320,7 @@
         <v>36</v>
       </c>
       <c r="AA27" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AB27" s="2"/>
       <c r="AC27" t="s" s="2">
@@ -3326,7 +3330,7 @@
         <v>62</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>39</v>
@@ -3343,10 +3347,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s" s="2">
         <v>36</v>
@@ -3368,13 +3372,13 @@
         <v>36</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -3425,7 +3429,7 @@
         <v>36</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>39</v>
@@ -3442,7 +3446,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -3465,11 +3469,11 @@
         <v>36</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -3518,7 +3522,7 @@
         <v>62</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>39</v>
@@ -3535,10 +3539,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>36</v>
@@ -3560,13 +3564,13 @@
         <v>36</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -3617,7 +3621,7 @@
         <v>36</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -3629,12 +3633,12 @@
         <v>36</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -3657,13 +3661,13 @@
         <v>36</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -3714,7 +3718,7 @@
         <v>36</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>39</v>
@@ -3731,7 +3735,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -3754,13 +3758,13 @@
         <v>36</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -3811,7 +3815,7 @@
         <v>36</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>39</v>
@@ -3828,7 +3832,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -3851,7 +3855,7 @@
         <v>36</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -3904,7 +3908,7 @@
         <v>36</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>39</v>
@@ -3921,7 +3925,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -3944,11 +3948,11 @@
         <v>36</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -3987,7 +3991,7 @@
         <v>36</v>
       </c>
       <c r="AA34" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AB34" s="2"/>
       <c r="AC34" t="s" s="2">
@@ -3997,7 +4001,7 @@
         <v>62</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>39</v>
@@ -4014,10 +4018,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C35" t="s" s="2">
         <v>36</v>
@@ -4039,13 +4043,13 @@
         <v>36</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -4096,7 +4100,7 @@
         <v>36</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>39</v>
@@ -4113,7 +4117,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4136,13 +4140,13 @@
         <v>36</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -4193,7 +4197,7 @@
         <v>36</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>39</v>
@@ -4210,7 +4214,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -4233,7 +4237,7 @@
         <v>36</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -4286,7 +4290,7 @@
         <v>36</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>37</v>

</xml_diff>